<commit_message>
slight change to spreadsheet
</commit_message>
<xml_diff>
--- a/model/System Model/System Model.xlsx
+++ b/model/System Model/System Model.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt\Documents\IIB Project\System Model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt\Documents\iib-project\model\System Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{189301D1-0170-43BE-A3D1-ABB88037BFA2}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{705B8F22-4321-4E76-92A2-1C1D9EFE19E0}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="2" xr2:uid="{2E20499A-CF7D-441A-9B23-3C755E67DBA1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{2E20499A-CF7D-441A-9B23-3C755E67DBA1}"/>
   </bookViews>
   <sheets>
     <sheet name="System Blocks" sheetId="2" r:id="rId1"/>
@@ -805,15 +805,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1055,15 +1046,6 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1173,9 +1155,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1227,64 +1206,85 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="8" fillId="4" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="8" fillId="7" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="8" fillId="2" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="8" fillId="4" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="8" fillId="7" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="8" fillId="2" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3502,18 +3502,18 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="173" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
+      <c r="E2" s="174"/>
+      <c r="F2" s="174"/>
+      <c r="G2" s="174"/>
     </row>
     <row r="3" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
+      <c r="D3" s="174"/>
+      <c r="E3" s="174"/>
+      <c r="F3" s="174"/>
+      <c r="G3" s="174"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3529,8 +3529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C58272F-101F-4B99-AF78-72AA6E441E3F}">
   <dimension ref="B2:H28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3542,27 +3542,27 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="175" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
+      <c r="C2" s="175"/>
+      <c r="D2" s="175"/>
     </row>
     <row r="3" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="1"/>
       <c r="D3"/>
     </row>
     <row r="4" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="71" t="s">
+      <c r="F4" s="68" t="s">
         <v>8</v>
       </c>
       <c r="G4" s="2" t="s">
@@ -3573,486 +3573,489 @@
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="27">
+      <c r="C5" s="24">
         <v>100</v>
       </c>
-      <c r="D5" s="28">
+      <c r="D5" s="25">
         <v>100</v>
       </c>
-      <c r="F5" s="72">
+      <c r="F5" s="69">
         <v>100</v>
       </c>
-      <c r="G5" s="80">
+      <c r="G5" s="77">
         <v>100</v>
       </c>
-      <c r="H5" s="28">
+      <c r="H5" s="25">
         <v>100</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="29">
+      <c r="C6" s="26">
         <f>10*LOG(C5,10)</f>
         <v>20</v>
       </c>
-      <c r="D6" s="25">
+      <c r="D6" s="22">
         <f>10*LOG(D5,10)</f>
         <v>20</v>
       </c>
-      <c r="F6" s="73">
+      <c r="F6" s="70">
         <f>10*LOG(F5,10)</f>
         <v>20</v>
       </c>
-      <c r="G6" s="81">
+      <c r="G6" s="78">
         <f>10*LOG(G5,10)</f>
         <v>20</v>
       </c>
-      <c r="H6" s="25">
+      <c r="H6" s="22">
         <f>10*LOG(H5,10)</f>
         <v>20</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="30">
+      <c r="C7" s="27">
         <v>3</v>
       </c>
-      <c r="D7" s="20">
+      <c r="D7" s="17">
         <v>3</v>
       </c>
-      <c r="F7" s="74">
+      <c r="F7" s="71">
         <v>3</v>
       </c>
-      <c r="G7" s="82">
+      <c r="G7" s="79">
         <v>3</v>
       </c>
-      <c r="H7" s="20">
+      <c r="H7" s="17">
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="30">
+      <c r="C8" s="27">
         <v>1</v>
       </c>
-      <c r="D8" s="20">
+      <c r="D8" s="17">
         <v>1</v>
       </c>
-      <c r="F8" s="74">
+      <c r="F8" s="71">
         <v>1</v>
       </c>
-      <c r="G8" s="82">
+      <c r="G8" s="79">
         <v>1</v>
       </c>
-      <c r="H8" s="20">
+      <c r="H8" s="17">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="31">
+      <c r="C9" s="28">
         <f>C6+C7-C8</f>
         <v>22</v>
       </c>
-      <c r="D9" s="21">
+      <c r="D9" s="18">
         <f>D6+D7-D8</f>
         <v>22</v>
       </c>
-      <c r="F9" s="75">
+      <c r="F9" s="72">
         <f>F6+F7-F8</f>
         <v>22</v>
       </c>
-      <c r="G9" s="83">
+      <c r="G9" s="80">
         <f>G6+G7-G8</f>
         <v>22</v>
       </c>
-      <c r="H9" s="21">
+      <c r="H9" s="18">
         <f>H6+H7-H8</f>
         <v>22</v>
       </c>
     </row>
     <row r="10" spans="2:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="30"/>
-      <c r="D10" s="20"/>
-      <c r="F10" s="74"/>
-      <c r="G10" s="82"/>
-      <c r="H10" s="20"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="17"/>
+      <c r="F10" s="71"/>
+      <c r="G10" s="79"/>
+      <c r="H10" s="17"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="27">
+      <c r="C11" s="24">
         <v>1</v>
       </c>
-      <c r="D11" s="28">
+      <c r="D11" s="25">
         <v>30</v>
       </c>
-      <c r="F11" s="72">
+      <c r="F11" s="69">
         <v>25.617000000000001</v>
       </c>
-      <c r="G11" s="80">
+      <c r="G11" s="77">
         <v>25.821000000000002</v>
       </c>
-      <c r="H11" s="28">
+      <c r="H11" s="25">
         <v>25.597000000000001</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="30">
+      <c r="C12" s="27">
         <v>2400</v>
       </c>
-      <c r="D12" s="20">
+      <c r="D12" s="17">
         <v>2400</v>
       </c>
-      <c r="F12" s="74">
+      <c r="F12" s="71">
         <v>2400</v>
       </c>
-      <c r="G12" s="82">
+      <c r="G12" s="79">
         <v>2400</v>
       </c>
-      <c r="H12" s="20">
+      <c r="H12" s="17">
         <v>2400</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="32">
+      <c r="C13" s="29">
         <f>20*LOG10(C11*1000)+20*LOG10(C12*1000000)-147.558</f>
         <v>100.04622483423213</v>
       </c>
-      <c r="D13" s="33">
+      <c r="D13" s="30">
         <f>20*LOG10(D11*1000)+20*LOG10(D12*1000000)-147.558</f>
         <v>129.58864992862539</v>
       </c>
-      <c r="F13" s="76">
+      <c r="F13" s="73">
         <f>20*LOG10(F11*1000)+20*LOG10(F12*1000000)-147.558</f>
         <v>128.21679019975687</v>
       </c>
-      <c r="G13" s="84">
+      <c r="G13" s="81">
         <f>20*LOG10(G11*1000)+20*LOG10(G12*1000000)-147.558</f>
         <v>128.28568598793856</v>
       </c>
-      <c r="H13" s="33">
+      <c r="H13" s="30">
         <f>20*LOG10(H11*1000)+20*LOG10(H12*1000000)-147.558</f>
         <v>128.21000620313123</v>
       </c>
     </row>
     <row r="14" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C14" s="34">
+      <c r="C14" s="31">
         <v>0</v>
       </c>
-      <c r="D14" s="35">
+      <c r="D14" s="32">
         <v>0</v>
       </c>
-      <c r="F14" s="77">
+      <c r="F14" s="74">
         <v>0</v>
       </c>
-      <c r="G14" s="85">
+      <c r="G14" s="82">
         <v>0</v>
       </c>
-      <c r="H14" s="35">
+      <c r="H14" s="32">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="2:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="36"/>
-      <c r="D15" s="24"/>
-      <c r="F15" s="78"/>
-      <c r="G15" s="86"/>
-      <c r="H15" s="24"/>
+      <c r="C15" s="33"/>
+      <c r="D15" s="21"/>
+      <c r="F15" s="75"/>
+      <c r="G15" s="83"/>
+      <c r="H15" s="21"/>
     </row>
     <row r="16" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="29">
+      <c r="C16" s="26">
         <f>C9-C13</f>
         <v>-78.046224834232135</v>
       </c>
-      <c r="D16" s="25">
+      <c r="D16" s="22">
         <f>D9-D13</f>
         <v>-107.58864992862539</v>
       </c>
-      <c r="F16" s="73">
+      <c r="F16" s="70">
         <f>F9-F13</f>
         <v>-106.21679019975687</v>
       </c>
-      <c r="G16" s="81">
+      <c r="G16" s="78">
         <f>G9-G13</f>
         <v>-106.28568598793856</v>
       </c>
-      <c r="H16" s="25">
+      <c r="H16" s="22">
         <f>H9-H13</f>
         <v>-106.21000620313123</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="30">
+      <c r="C17" s="27">
         <v>16</v>
       </c>
-      <c r="D17" s="20">
+      <c r="D17" s="17">
         <v>16</v>
       </c>
-      <c r="F17" s="74">
+      <c r="F17" s="71">
         <v>16</v>
       </c>
-      <c r="G17" s="82">
+      <c r="G17" s="79">
         <v>16</v>
       </c>
-      <c r="H17" s="20">
+      <c r="H17" s="17">
         <v>16</v>
       </c>
     </row>
     <row r="18" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="29">
+      <c r="C18" s="26">
         <f>C16+C17</f>
         <v>-62.046224834232135</v>
       </c>
-      <c r="D18" s="25">
+      <c r="D18" s="22">
         <f>D16+D17</f>
         <v>-91.588649928625387</v>
       </c>
-      <c r="F18" s="73">
+      <c r="F18" s="70">
         <f>F16+F17</f>
         <v>-90.216790199756872</v>
       </c>
-      <c r="G18" s="81">
+      <c r="G18" s="78">
         <f>G16+G17</f>
         <v>-90.285685987938564</v>
       </c>
-      <c r="H18" s="25">
+      <c r="H18" s="22">
         <f>H16+H17</f>
         <v>-90.210006203131229</v>
       </c>
     </row>
     <row r="19" spans="2:8" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="36"/>
-      <c r="D19" s="24"/>
-      <c r="F19" s="78"/>
-      <c r="G19" s="86"/>
-      <c r="H19" s="24"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="21"/>
+      <c r="F19" s="75"/>
+      <c r="G19" s="83"/>
+      <c r="H19" s="21"/>
     </row>
     <row r="20" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="29">
+      <c r="C20" s="26">
         <f>C18</f>
         <v>-62.046224834232135</v>
       </c>
-      <c r="D20" s="25">
+      <c r="D20" s="22">
         <f>D18</f>
         <v>-91.588649928625387</v>
       </c>
-      <c r="F20" s="73">
+      <c r="F20" s="70">
         <f>F18</f>
         <v>-90.216790199756872</v>
       </c>
-      <c r="G20" s="81">
+      <c r="G20" s="78">
         <f>G18</f>
         <v>-90.285685987938564</v>
       </c>
-      <c r="H20" s="25">
+      <c r="H20" s="22">
         <f>H18</f>
         <v>-90.210006203131229</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="30">
+      <c r="C21" s="27">
         <v>23</v>
       </c>
-      <c r="D21" s="20">
+      <c r="D21" s="17">
         <v>23</v>
       </c>
-      <c r="F21" s="74">
+      <c r="F21" s="71">
         <v>23</v>
       </c>
-      <c r="G21" s="82">
+      <c r="G21" s="79">
         <v>23</v>
       </c>
-      <c r="H21" s="20">
+      <c r="H21" s="17">
         <v>23</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="11" t="s">
+      <c r="B22" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C22" s="30">
+      <c r="C22" s="27">
         <v>1.6</v>
       </c>
-      <c r="D22" s="20">
+      <c r="D22" s="17">
         <v>1.6</v>
       </c>
-      <c r="F22" s="74">
+      <c r="F22" s="71">
         <v>1.6</v>
       </c>
-      <c r="G22" s="82">
+      <c r="G22" s="79">
         <v>1.6</v>
       </c>
-      <c r="H22" s="20">
+      <c r="H22" s="17">
         <v>1.6</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="11" t="s">
+      <c r="B23" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="30">
+      <c r="C23" s="27">
         <v>1</v>
       </c>
-      <c r="D23" s="20">
+      <c r="D23" s="17">
         <v>1</v>
       </c>
-      <c r="F23" s="74">
+      <c r="F23" s="71">
         <v>1</v>
       </c>
-      <c r="G23" s="82">
+      <c r="G23" s="79">
         <v>1</v>
       </c>
-      <c r="H23" s="20">
+      <c r="H23" s="17">
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="16" t="s">
+      <c r="B24" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="29">
+      <c r="C24" s="26">
         <f>C20+C21-C22-C23</f>
         <v>-41.646224834232136</v>
       </c>
-      <c r="D24" s="25">
+      <c r="D24" s="22">
         <f>D20+D21-D22-D23</f>
         <v>-71.188649928625381</v>
       </c>
-      <c r="F24" s="73">
+      <c r="F24" s="70">
         <f>F20+F21-F22-F23</f>
         <v>-69.816790199756866</v>
       </c>
-      <c r="G24" s="81">
+      <c r="G24" s="78">
         <f>G20+G21-G22-G23</f>
         <v>-69.885685987938558</v>
       </c>
-      <c r="H24" s="25">
+      <c r="H24" s="22">
         <f>H20+H21-H22-H23</f>
         <v>-69.810006203131223</v>
       </c>
     </row>
     <row r="25" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="15" t="s">
+      <c r="B25" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="C25" s="36"/>
-      <c r="D25" s="24"/>
-      <c r="F25" s="78"/>
-      <c r="G25" s="86"/>
-      <c r="H25" s="24"/>
+      <c r="C25" s="33"/>
+      <c r="D25" s="21"/>
+      <c r="F25" s="75"/>
+      <c r="G25" s="83"/>
+      <c r="H25" s="21"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="16" t="s">
+      <c r="B26" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C26" s="29">
+      <c r="C26" s="26">
         <f>C24</f>
         <v>-41.646224834232136</v>
       </c>
-      <c r="D26" s="25">
+      <c r="D26" s="22">
         <f>D24</f>
         <v>-71.188649928625381</v>
       </c>
-      <c r="F26" s="73">
+      <c r="F26" s="70">
         <f>F24</f>
         <v>-69.816790199756866</v>
       </c>
-      <c r="G26" s="81">
+      <c r="G26" s="78">
         <f>G24</f>
         <v>-69.885685987938558</v>
       </c>
-      <c r="H26" s="25">
+      <c r="H26" s="22">
         <f>H24</f>
         <v>-69.810006203131223</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B27" s="14" t="s">
+      <c r="B27" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C27" s="30">
+      <c r="C27" s="27">
         <v>55</v>
       </c>
-      <c r="D27" s="20">
+      <c r="D27" s="17">
         <v>55</v>
       </c>
-      <c r="F27" s="74">
+      <c r="F27" s="71">
+        <f>D27</f>
         <v>55</v>
       </c>
-      <c r="G27" s="82">
+      <c r="G27" s="79">
+        <f>D27</f>
         <v>55</v>
       </c>
-      <c r="H27" s="20">
+      <c r="H27" s="17">
+        <f>D27</f>
         <v>55</v>
       </c>
     </row>
     <row r="28" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="17" t="s">
+      <c r="B28" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C28" s="37">
+      <c r="C28" s="34">
         <f>C26+C27</f>
         <v>13.353775165767864</v>
       </c>
-      <c r="D28" s="26">
+      <c r="D28" s="23">
         <f>D26+D27</f>
         <v>-16.188649928625381</v>
       </c>
-      <c r="F28" s="79">
+      <c r="F28" s="76">
         <f>F26+F27</f>
         <v>-14.816790199756866</v>
       </c>
-      <c r="G28" s="87">
+      <c r="G28" s="84">
         <f>G26+G27</f>
         <v>-14.885685987938558</v>
       </c>
-      <c r="H28" s="26">
+      <c r="H28" s="23">
         <f>H26+H27</f>
         <v>-14.810006203131223</v>
       </c>
@@ -4070,8 +4073,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E61DD661-5A70-43C1-A29A-3078B8E22ACC}">
   <dimension ref="B2:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4088,384 +4091,385 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="I2" s="161" t="s">
+      <c r="I2" s="176" t="s">
         <v>54</v>
       </c>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
+      <c r="J2" s="174"/>
+      <c r="K2" s="174"/>
+      <c r="L2" s="174"/>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
+      <c r="I3" s="174"/>
+      <c r="J3" s="174"/>
+      <c r="K3" s="174"/>
+      <c r="L3" s="174"/>
     </row>
     <row r="4" spans="2:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="58" t="s">
+      <c r="B4" s="55" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="58"/>
-      <c r="D4" s="58"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
     </row>
     <row r="5" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="22"/>
-      <c r="D5" s="48"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="23"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="20"/>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="54">
+      <c r="C6" s="51">
         <f>POWER(10, 0.1*E6)</f>
         <v>199.52623149688819</v>
       </c>
-      <c r="D6" s="49"/>
-      <c r="E6" s="18">
+      <c r="D6" s="46"/>
+      <c r="E6" s="15">
         <v>23</v>
       </c>
-      <c r="F6" s="20" t="s">
+      <c r="F6" s="17" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="54">
+      <c r="C7" s="51">
         <f>POWER(10, 0.1*E7)</f>
         <v>1.8281002161427427</v>
       </c>
-      <c r="D7" s="49"/>
-      <c r="E7" s="18">
+      <c r="D7" s="46"/>
+      <c r="E7" s="15">
         <v>2.62</v>
       </c>
-      <c r="F7" s="20" t="s">
+      <c r="F7" s="17" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="8" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="55">
+      <c r="C8" s="52">
         <f>290*(C7-1)</f>
         <v>240.14906268139538</v>
       </c>
-      <c r="D8" s="50" t="s">
+      <c r="D8" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="40"/>
-      <c r="F8" s="41"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="38"/>
     </row>
     <row r="9" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="56"/>
-      <c r="D9" s="48"/>
-      <c r="E9" s="47"/>
-      <c r="F9" s="23"/>
+      <c r="C9" s="53"/>
+      <c r="D9" s="45"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="20"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="54">
+      <c r="C10" s="51">
         <f>POWER(10, 0.1*E10)</f>
         <v>0.69183097091893642</v>
       </c>
-      <c r="D10" s="49"/>
-      <c r="E10" s="18">
+      <c r="D10" s="46"/>
+      <c r="E10" s="15">
         <v>-1.6</v>
       </c>
-      <c r="F10" s="19" t="s">
+      <c r="F10" s="16" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="54">
+      <c r="C11" s="51">
         <f>POWER(10, 0.1*E11)</f>
         <v>1.4454397707459277</v>
       </c>
-      <c r="D11" s="49"/>
-      <c r="E11" s="18">
+      <c r="D11" s="46"/>
+      <c r="E11" s="15">
         <v>1.6</v>
       </c>
-      <c r="F11" s="19" t="s">
+      <c r="F11" s="16" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="12" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="55">
+      <c r="C12" s="52">
         <f>290*(C11-1)</f>
         <v>129.17753351631902</v>
       </c>
-      <c r="D12" s="50" t="s">
+      <c r="D12" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="40"/>
-      <c r="F12" s="41"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="38"/>
     </row>
     <row r="13" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="56"/>
-      <c r="D13" s="48"/>
-      <c r="E13" s="47"/>
-      <c r="F13" s="23"/>
+      <c r="C13" s="53"/>
+      <c r="D13" s="45"/>
+      <c r="E13" s="44"/>
+      <c r="F13" s="20"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="54">
+      <c r="C14" s="51">
         <f>POWER(10, 0.1*E14)</f>
         <v>316227.7660168382</v>
       </c>
-      <c r="D14" s="49"/>
-      <c r="E14" s="18">
+      <c r="D14" s="46"/>
+      <c r="E14" s="15">
+        <f>'Link Budget'!D27</f>
         <v>55</v>
       </c>
-      <c r="F14" s="19" t="s">
+      <c r="F14" s="16" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="54">
+      <c r="C15" s="51">
         <f>POWER(10, 0.1*E15)</f>
         <v>2.2387211385683399</v>
       </c>
-      <c r="D15" s="49"/>
-      <c r="E15" s="18">
+      <c r="D15" s="46"/>
+      <c r="E15" s="15">
         <v>3.5</v>
       </c>
-      <c r="F15" s="19" t="s">
+      <c r="F15" s="16" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="16" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="57">
+      <c r="C16" s="54">
         <f>290*(C15-1)</f>
         <v>359.22913018481859</v>
       </c>
-      <c r="D16" s="51" t="s">
+      <c r="D16" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="E16" s="42"/>
-      <c r="F16" s="43"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="40"/>
     </row>
     <row r="19" spans="2:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="58" t="s">
+      <c r="B19" s="55" t="s">
         <v>56</v>
       </c>
-      <c r="C19" s="58"/>
-      <c r="D19" s="58"/>
+      <c r="C19" s="55"/>
+      <c r="D19" s="55"/>
     </row>
     <row r="20" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="22"/>
-      <c r="D20" s="48"/>
-      <c r="E20" s="47"/>
-      <c r="F20" s="23"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="45"/>
+      <c r="E20" s="44"/>
+      <c r="F20" s="20"/>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B21" s="16" t="s">
+      <c r="B21" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="55">
+      <c r="C21" s="52">
         <f>POWER(10, 0.1*E21)</f>
         <v>43651583.224016666</v>
       </c>
-      <c r="D21" s="50"/>
-      <c r="E21" s="55">
+      <c r="D21" s="47"/>
+      <c r="E21" s="52">
         <f>E6+E10+E14</f>
         <v>76.400000000000006</v>
       </c>
-      <c r="F21" s="41" t="s">
+      <c r="F21" s="38" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B22" s="67" t="s">
+      <c r="B22" s="64" t="s">
         <v>31</v>
       </c>
-      <c r="C22" s="68">
+      <c r="C22" s="65">
         <f>C7+((C11-1)/C6)+((C15-1)/(C10*C6))</f>
         <v>1.8393064447800593</v>
       </c>
-      <c r="D22" s="69"/>
-      <c r="E22" s="68">
+      <c r="D22" s="66"/>
+      <c r="E22" s="65">
         <f>10*LOG10(C22)</f>
         <v>2.6465409258207488</v>
       </c>
-      <c r="F22" s="70" t="s">
+      <c r="F22" s="67" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="23" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="17" t="s">
+      <c r="B23" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="C23" s="57">
+      <c r="C23" s="54">
         <f>290*(C22-1)</f>
         <v>243.3988689862172</v>
       </c>
-      <c r="D23" s="51" t="s">
+      <c r="D23" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="E23" s="42"/>
-      <c r="F23" s="43"/>
+      <c r="E23" s="39"/>
+      <c r="F23" s="40"/>
     </row>
     <row r="26" spans="2:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="58" t="s">
+      <c r="B26" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="C26" s="88"/>
-      <c r="D26" s="88"/>
-      <c r="E26" s="38"/>
-      <c r="F26" s="38"/>
-      <c r="I26" s="162" t="s">
+      <c r="C26" s="85"/>
+      <c r="D26" s="85"/>
+      <c r="E26" s="35"/>
+      <c r="F26" s="35"/>
+      <c r="I26" s="154" t="s">
         <v>55</v>
       </c>
-      <c r="J26" s="162"/>
-      <c r="K26" s="162"/>
+      <c r="J26" s="154"/>
+      <c r="K26" s="154"/>
     </row>
     <row r="27" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="52" t="s">
+      <c r="B27" s="49" t="s">
         <v>40</v>
       </c>
-      <c r="C27" s="60"/>
-      <c r="D27" s="44"/>
-      <c r="E27" s="53"/>
-      <c r="F27" s="45"/>
-      <c r="I27" s="97" t="s">
+      <c r="C27" s="57"/>
+      <c r="D27" s="41"/>
+      <c r="E27" s="50"/>
+      <c r="F27" s="42"/>
+      <c r="I27" s="94" t="s">
         <v>11</v>
       </c>
-      <c r="J27" s="98" t="s">
+      <c r="J27" s="95" t="s">
         <v>42</v>
       </c>
-      <c r="K27" s="97" t="s">
+      <c r="K27" s="94" t="s">
         <v>43</v>
       </c>
-      <c r="L27" s="99" t="s">
+      <c r="L27" s="96" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B28" s="10" t="s">
+      <c r="B28" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C28" s="65">
+      <c r="C28" s="62">
         <v>290</v>
       </c>
-      <c r="D28" s="61" t="s">
+      <c r="D28" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="E28" s="62"/>
-      <c r="F28" s="46"/>
-      <c r="I28" s="93">
+      <c r="E28" s="59"/>
+      <c r="F28" s="43"/>
+      <c r="I28" s="90">
         <v>1</v>
       </c>
-      <c r="J28" s="100">
+      <c r="J28" s="97">
         <f>'Link Budget'!F28</f>
         <v>-14.816790199756866</v>
       </c>
-      <c r="K28" s="95">
+      <c r="K28" s="92">
         <f>E30</f>
         <v>-23.169775640620504</v>
       </c>
-      <c r="L28" s="101">
+      <c r="L28" s="98">
         <f>J28-K28</f>
         <v>8.3529854408636375</v>
       </c>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B29" s="11" t="s">
+      <c r="B29" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C29" s="91">
+      <c r="C29" s="88">
         <f>(1.38E-23)*C28*15000000*1000</f>
         <v>6.0030000000000011E-11</v>
       </c>
-      <c r="D29" s="89" t="s">
+      <c r="D29" s="86" t="s">
         <v>16</v>
       </c>
-      <c r="E29" s="92">
+      <c r="E29" s="89">
         <f>10*LOG10(C29)</f>
         <v>-102.21631656644126</v>
       </c>
-      <c r="F29" s="90" t="s">
+      <c r="F29" s="87" t="s">
         <v>17</v>
       </c>
-      <c r="I29" s="93">
+      <c r="I29" s="90">
         <v>2</v>
       </c>
-      <c r="J29" s="100">
+      <c r="J29" s="97">
         <f>'Link Budget'!G28</f>
         <v>-14.885685987938558</v>
       </c>
-      <c r="K29" s="95">
+      <c r="K29" s="92">
         <f>E30</f>
         <v>-23.169775640620504</v>
       </c>
-      <c r="L29" s="101">
+      <c r="L29" s="98">
         <f t="shared" ref="L29:L30" si="0">J29-K29</f>
         <v>8.2840896526819456</v>
       </c>
     </row>
     <row r="30" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="12" t="s">
+      <c r="B30" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C30" s="66">
+      <c r="C30" s="63">
         <f>(1.38E-23)*(C28+C23)*15000000*C21*1000</f>
         <v>4.8197269600776822E-3</v>
       </c>
-      <c r="D30" s="63" t="s">
+      <c r="D30" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="E30" s="64">
+      <c r="E30" s="61">
         <f>10*LOG10(C30)</f>
         <v>-23.169775640620504</v>
       </c>
-      <c r="F30" s="59" t="s">
+      <c r="F30" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="I30" s="94">
+      <c r="I30" s="91">
         <v>3</v>
       </c>
-      <c r="J30" s="63">
+      <c r="J30" s="60">
         <f>'Link Budget'!H28</f>
         <v>-14.810006203131223</v>
       </c>
-      <c r="K30" s="96">
+      <c r="K30" s="93">
         <f>E30</f>
         <v>-23.169775640620504</v>
       </c>
-      <c r="L30" s="102">
+      <c r="L30" s="99">
         <f t="shared" si="0"/>
         <v>8.3597694374892804</v>
       </c>
@@ -4499,620 +4503,620 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="143" t="s">
+      <c r="B1" s="180" t="s">
         <v>50</v>
       </c>
-      <c r="C1" s="143"/>
-      <c r="D1" s="143"/>
-      <c r="E1" s="143"/>
-      <c r="F1" s="143"/>
-      <c r="G1" s="143"/>
-      <c r="J1" s="143" t="s">
+      <c r="C1" s="180"/>
+      <c r="D1" s="180"/>
+      <c r="E1" s="180"/>
+      <c r="F1" s="180"/>
+      <c r="G1" s="180"/>
+      <c r="J1" s="180" t="s">
         <v>51</v>
       </c>
-      <c r="K1" s="143"/>
-      <c r="L1" s="143"/>
-      <c r="M1" s="143"/>
-      <c r="N1" s="143"/>
-      <c r="O1" s="143"/>
+      <c r="K1" s="180"/>
+      <c r="L1" s="180"/>
+      <c r="M1" s="180"/>
+      <c r="N1" s="180"/>
+      <c r="O1" s="180"/>
     </row>
     <row r="2" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="143"/>
-      <c r="C2" s="143"/>
-      <c r="D2" s="143"/>
-      <c r="E2" s="143"/>
-      <c r="F2" s="143"/>
-      <c r="G2" s="143"/>
-      <c r="J2" s="143"/>
-      <c r="K2" s="143"/>
-      <c r="L2" s="143"/>
-      <c r="M2" s="143"/>
-      <c r="N2" s="143"/>
-      <c r="O2" s="143"/>
+      <c r="B2" s="180"/>
+      <c r="C2" s="180"/>
+      <c r="D2" s="180"/>
+      <c r="E2" s="180"/>
+      <c r="F2" s="180"/>
+      <c r="G2" s="180"/>
+      <c r="J2" s="180"/>
+      <c r="K2" s="180"/>
+      <c r="L2" s="180"/>
+      <c r="M2" s="180"/>
+      <c r="N2" s="180"/>
+      <c r="O2" s="180"/>
     </row>
     <row r="3" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E4" s="103" t="s">
+      <c r="E4" s="177" t="s">
         <v>49</v>
       </c>
-      <c r="F4" s="104"/>
-      <c r="G4" s="105"/>
+      <c r="F4" s="178"/>
+      <c r="G4" s="179"/>
       <c r="J4" s="4"/>
-      <c r="K4" s="103" t="s">
+      <c r="K4" s="177" t="s">
         <v>49</v>
       </c>
-      <c r="L4" s="104"/>
-      <c r="M4" s="105"/>
+      <c r="L4" s="178"/>
+      <c r="M4" s="179"/>
     </row>
     <row r="5" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="106" t="s">
+      <c r="B5" s="100" t="s">
         <v>44</v>
       </c>
-      <c r="C5" s="108" t="s">
+      <c r="C5" s="102" t="s">
         <v>45</v>
       </c>
-      <c r="D5" s="107" t="s">
+      <c r="D5" s="101" t="s">
         <v>42</v>
       </c>
-      <c r="E5" s="106" t="s">
+      <c r="E5" s="100" t="s">
         <v>48</v>
       </c>
-      <c r="F5" s="108" t="s">
+      <c r="F5" s="102" t="s">
         <v>47</v>
       </c>
-      <c r="G5" s="107" t="s">
+      <c r="G5" s="101" t="s">
         <v>46</v>
       </c>
-      <c r="J5" s="151" t="s">
+      <c r="J5" s="144" t="s">
         <v>45</v>
       </c>
-      <c r="K5" s="106" t="s">
+      <c r="K5" s="100" t="s">
         <v>48</v>
       </c>
-      <c r="L5" s="108" t="s">
+      <c r="L5" s="102" t="s">
         <v>47</v>
       </c>
-      <c r="M5" s="107" t="s">
+      <c r="M5" s="101" t="s">
         <v>46</v>
       </c>
-      <c r="N5" s="157" t="s">
+      <c r="N5" s="150" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B6" s="163">
+      <c r="B6" s="155">
         <v>-60</v>
       </c>
-      <c r="C6" s="164">
+      <c r="C6" s="156">
         <v>65</v>
       </c>
-      <c r="D6" s="165">
+      <c r="D6" s="157">
         <f t="shared" ref="D6" si="0">B6+C6</f>
         <v>5</v>
       </c>
-      <c r="E6" s="166">
+      <c r="E6" s="158">
         <v>500223</v>
       </c>
-      <c r="F6" s="167">
+      <c r="F6" s="159">
         <f t="shared" ref="F6:F15" si="1">10*LOG10(E6)</f>
         <v>56.991636564937252</v>
       </c>
-      <c r="G6" s="168">
+      <c r="G6" s="160">
         <v>1211</v>
       </c>
-      <c r="J6" s="152">
+      <c r="J6" s="145">
         <v>73</v>
       </c>
-      <c r="K6" s="148">
+      <c r="K6" s="141">
         <v>838</v>
       </c>
-      <c r="L6" s="149">
+      <c r="L6" s="142">
         <f t="shared" ref="L6:L10" si="2">10*LOG10(K6)</f>
         <v>29.232440186302764</v>
       </c>
-      <c r="M6" s="150">
+      <c r="M6" s="143">
         <v>150</v>
       </c>
-      <c r="N6" s="95">
+      <c r="N6" s="92">
         <f>(L6-52.9106)/0.9767</f>
         <v>-24.24302223169575</v>
       </c>
-      <c r="O6" s="159">
+      <c r="O6" s="152">
         <f>N6-J6</f>
         <v>-97.243022231695747</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B7" s="109">
+      <c r="B7" s="103">
         <v>-60</v>
       </c>
-      <c r="C7" s="110">
+      <c r="C7" s="104">
         <v>60</v>
       </c>
-      <c r="D7" s="111">
+      <c r="D7" s="105">
         <f>B7+C7</f>
         <v>0</v>
       </c>
-      <c r="E7" s="112">
+      <c r="E7" s="106">
         <v>205969</v>
       </c>
-      <c r="F7" s="113">
+      <c r="F7" s="107">
         <f>10*LOG10(E7)</f>
         <v>53.138018604563229</v>
       </c>
-      <c r="G7" s="114">
+      <c r="G7" s="108">
         <v>672</v>
       </c>
-      <c r="J7" s="152">
+      <c r="J7" s="145">
         <v>70</v>
       </c>
-      <c r="K7" s="148">
+      <c r="K7" s="141">
         <v>355</v>
       </c>
-      <c r="L7" s="149">
+      <c r="L7" s="142">
         <f>10*LOG10(K7)</f>
         <v>25.50228353055094</v>
       </c>
-      <c r="M7" s="150">
+      <c r="M7" s="143">
         <v>105</v>
       </c>
-      <c r="N7" s="95">
+      <c r="N7" s="92">
         <f t="shared" ref="N7:N11" si="3">(L7-52.9106)/0.9767</f>
         <v>-28.062164911896243</v>
       </c>
-      <c r="O7" s="95">
+      <c r="O7" s="92">
         <f t="shared" ref="O7:O11" si="4">N7-J7</f>
         <v>-98.062164911896247</v>
       </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B8" s="115">
+      <c r="B8" s="109">
         <v>-60</v>
       </c>
-      <c r="C8" s="116">
+      <c r="C8" s="110">
         <v>55</v>
       </c>
-      <c r="D8" s="117">
+      <c r="D8" s="111">
         <f>B8+C8</f>
         <v>-5</v>
       </c>
-      <c r="E8" s="118">
+      <c r="E8" s="112">
         <v>65946</v>
       </c>
-      <c r="F8" s="119">
+      <c r="F8" s="113">
         <f>10*LOG10(E8)</f>
         <v>48.191884582506717</v>
       </c>
-      <c r="G8" s="120">
+      <c r="G8" s="114">
         <v>380</v>
       </c>
-      <c r="J8" s="152">
+      <c r="J8" s="145">
         <v>65</v>
       </c>
-      <c r="K8" s="148">
+      <c r="K8" s="141">
         <v>114</v>
       </c>
-      <c r="L8" s="149">
+      <c r="L8" s="142">
         <f>10*LOG10(K8)</f>
         <v>20.569048513364727</v>
       </c>
-      <c r="M8" s="150">
+      <c r="M8" s="143">
         <v>61</v>
       </c>
-      <c r="N8" s="95">
+      <c r="N8" s="92">
         <f t="shared" si="3"/>
         <v>-33.113086399749434</v>
       </c>
-      <c r="O8" s="95">
+      <c r="O8" s="92">
         <f t="shared" si="4"/>
         <v>-98.113086399749434</v>
       </c>
     </row>
     <row r="9" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="169">
+      <c r="B9" s="161">
         <v>-60</v>
       </c>
-      <c r="C9" s="170">
+      <c r="C9" s="162">
         <v>50</v>
       </c>
-      <c r="D9" s="171">
+      <c r="D9" s="163">
         <f>B9+C9</f>
         <v>-10</v>
       </c>
-      <c r="E9" s="172">
+      <c r="E9" s="164">
         <v>21740</v>
       </c>
-      <c r="F9" s="173">
+      <c r="F9" s="165">
         <f>10*LOG10(E9)</f>
         <v>43.372595397502764</v>
       </c>
-      <c r="G9" s="174">
+      <c r="G9" s="166">
         <v>220</v>
       </c>
-      <c r="J9" s="152">
+      <c r="J9" s="145">
         <v>60</v>
       </c>
-      <c r="K9" s="148">
+      <c r="K9" s="141">
         <v>49.5</v>
       </c>
-      <c r="L9" s="149">
+      <c r="L9" s="142">
         <f>10*LOG10(K9)</f>
         <v>16.946051989335686</v>
       </c>
-      <c r="M9" s="150">
+      <c r="M9" s="143">
         <v>37</v>
       </c>
-      <c r="N9" s="95">
+      <c r="N9" s="92">
         <f t="shared" si="3"/>
         <v>-36.822512553152777</v>
       </c>
-      <c r="O9" s="95">
+      <c r="O9" s="92">
         <f t="shared" si="4"/>
         <v>-96.822512553152777</v>
       </c>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B10" s="163">
+      <c r="B10" s="155">
         <v>-65</v>
       </c>
-      <c r="C10" s="164">
+      <c r="C10" s="156">
         <v>70</v>
       </c>
-      <c r="D10" s="165">
+      <c r="D10" s="157">
         <f t="shared" ref="D10" si="5">B10+C10</f>
         <v>5</v>
       </c>
-      <c r="E10" s="166">
+      <c r="E10" s="158">
         <v>636408</v>
       </c>
-      <c r="F10" s="167">
+      <c r="F10" s="159">
         <f t="shared" si="1"/>
         <v>58.037356303303227</v>
       </c>
-      <c r="G10" s="168">
+      <c r="G10" s="160">
         <v>1222</v>
       </c>
-      <c r="J10" s="152">
+      <c r="J10" s="145">
         <v>55</v>
       </c>
-      <c r="K10" s="148">
+      <c r="K10" s="141">
         <v>17</v>
       </c>
-      <c r="L10" s="149">
+      <c r="L10" s="142">
         <f t="shared" si="2"/>
         <v>12.304489213782739</v>
       </c>
-      <c r="M10" s="150">
+      <c r="M10" s="143">
         <v>21</v>
       </c>
-      <c r="N10" s="95">
+      <c r="N10" s="92">
         <f t="shared" si="3"/>
         <v>-41.574803712723728</v>
       </c>
-      <c r="O10" s="95">
+      <c r="O10" s="92">
         <f t="shared" si="4"/>
         <v>-96.574803712723735</v>
       </c>
     </row>
     <row r="11" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="109">
+      <c r="B11" s="103">
         <v>-65</v>
       </c>
-      <c r="C11" s="110">
+      <c r="C11" s="104">
         <v>65</v>
       </c>
-      <c r="D11" s="111">
+      <c r="D11" s="105">
         <v>0</v>
       </c>
-      <c r="E11" s="112">
+      <c r="E11" s="106">
         <v>212424</v>
       </c>
-      <c r="F11" s="113">
+      <c r="F11" s="107">
         <f>10*LOG10(E11)</f>
         <v>53.272035824599783</v>
       </c>
-      <c r="G11" s="114">
+      <c r="G11" s="108">
         <v>698</v>
       </c>
-      <c r="J11" s="153">
+      <c r="J11" s="146">
         <v>50</v>
       </c>
-      <c r="K11" s="154">
+      <c r="K11" s="147">
         <v>7.36</v>
       </c>
-      <c r="L11" s="155">
+      <c r="L11" s="148">
         <f>10*LOG10(K11)</f>
         <v>8.6687781433749898</v>
       </c>
-      <c r="M11" s="156">
+      <c r="M11" s="149">
         <v>13</v>
       </c>
-      <c r="N11" s="96">
+      <c r="N11" s="93">
         <f t="shared" si="3"/>
         <v>-45.297247728703809</v>
       </c>
-      <c r="O11" s="96">
+      <c r="O11" s="93">
         <f t="shared" si="4"/>
         <v>-95.297247728703809</v>
       </c>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B12" s="115">
+      <c r="B12" s="109">
         <v>-65</v>
       </c>
-      <c r="C12" s="116">
+      <c r="C12" s="110">
         <v>60</v>
       </c>
-      <c r="D12" s="117">
+      <c r="D12" s="111">
         <f>B12+C12</f>
         <v>-5</v>
       </c>
-      <c r="E12" s="118">
+      <c r="E12" s="112">
         <v>64371</v>
       </c>
-      <c r="F12" s="119">
+      <c r="F12" s="113">
         <f>10*LOG10(E12)</f>
         <v>48.086902559226388</v>
       </c>
-      <c r="G12" s="120">
+      <c r="G12" s="114">
         <v>391</v>
       </c>
-      <c r="J12" s="145"/>
-      <c r="K12" s="145"/>
-      <c r="L12" s="146"/>
-      <c r="M12" s="147"/>
-      <c r="N12" s="158" t="s">
+      <c r="J12" s="138"/>
+      <c r="K12" s="138"/>
+      <c r="L12" s="139"/>
+      <c r="M12" s="140"/>
+      <c r="N12" s="151" t="s">
         <v>53</v>
       </c>
-      <c r="O12" s="160">
+      <c r="O12" s="153">
         <f>AVERAGE(O6:O11)</f>
         <v>-97.018806256320275</v>
       </c>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B13" s="121">
+      <c r="B13" s="115">
         <v>-65</v>
       </c>
-      <c r="C13" s="122">
+      <c r="C13" s="116">
         <v>55</v>
       </c>
-      <c r="D13" s="123">
+      <c r="D13" s="117">
         <f>B13+C13</f>
         <v>-10</v>
       </c>
-      <c r="E13" s="124">
+      <c r="E13" s="118">
         <v>20630</v>
       </c>
-      <c r="F13" s="125">
+      <c r="F13" s="119">
         <f>10*LOG10(E13)</f>
         <v>43.144992279731518</v>
       </c>
-      <c r="G13" s="126">
+      <c r="G13" s="120">
         <v>220</v>
       </c>
-      <c r="J13" s="145"/>
-      <c r="K13" s="145"/>
-      <c r="L13" s="146"/>
-      <c r="M13" s="147"/>
+      <c r="J13" s="138"/>
+      <c r="K13" s="138"/>
+      <c r="L13" s="139"/>
+      <c r="M13" s="140"/>
     </row>
     <row r="14" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="175">
+      <c r="B14" s="167">
         <v>-65</v>
       </c>
-      <c r="C14" s="176">
+      <c r="C14" s="168">
         <v>50</v>
       </c>
-      <c r="D14" s="177">
+      <c r="D14" s="169">
         <f>B14+C14</f>
         <v>-15</v>
       </c>
-      <c r="E14" s="178">
+      <c r="E14" s="170">
         <v>6879</v>
       </c>
-      <c r="F14" s="179">
+      <c r="F14" s="171">
         <f>10*LOG10(E14)</f>
         <v>38.375253094496017</v>
       </c>
-      <c r="G14" s="180">
+      <c r="G14" s="172">
         <v>129</v>
       </c>
-      <c r="J14" s="145"/>
-      <c r="K14" s="145"/>
-      <c r="L14" s="146"/>
-      <c r="M14" s="147"/>
+      <c r="J14" s="138"/>
+      <c r="K14" s="138"/>
+      <c r="L14" s="139"/>
+      <c r="M14" s="140"/>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B15" s="109">
+      <c r="B15" s="103">
         <v>-70</v>
       </c>
-      <c r="C15" s="110">
+      <c r="C15" s="104">
         <v>70</v>
       </c>
-      <c r="D15" s="111">
+      <c r="D15" s="105">
         <f>B15+C15</f>
         <v>0</v>
       </c>
-      <c r="E15" s="112">
+      <c r="E15" s="106">
         <v>199693</v>
       </c>
-      <c r="F15" s="113">
+      <c r="F15" s="107">
         <f t="shared" si="1"/>
         <v>53.003628414623122</v>
       </c>
-      <c r="G15" s="114">
+      <c r="G15" s="108">
         <v>721</v>
       </c>
-      <c r="J15" s="145"/>
-      <c r="K15" s="145"/>
-      <c r="L15" s="146"/>
-      <c r="M15" s="147"/>
+      <c r="J15" s="138"/>
+      <c r="K15" s="138"/>
+      <c r="L15" s="139"/>
+      <c r="M15" s="140"/>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B16" s="115">
+      <c r="B16" s="109">
         <v>-70</v>
       </c>
-      <c r="C16" s="116">
+      <c r="C16" s="110">
         <v>65</v>
       </c>
-      <c r="D16" s="117">
+      <c r="D16" s="111">
         <f t="shared" ref="D16:D19" si="6">B16+C16</f>
         <v>-5</v>
       </c>
-      <c r="E16" s="118">
+      <c r="E16" s="112">
         <v>64219</v>
       </c>
-      <c r="F16" s="119">
+      <c r="F16" s="113">
         <f>10*LOG10(E16)</f>
         <v>48.076635385730057</v>
       </c>
-      <c r="G16" s="120">
+      <c r="G16" s="114">
         <v>418</v>
       </c>
-      <c r="J16" s="145"/>
-      <c r="K16" s="145"/>
-      <c r="L16" s="146"/>
-      <c r="M16" s="147"/>
+      <c r="J16" s="138"/>
+      <c r="K16" s="138"/>
+      <c r="L16" s="139"/>
+      <c r="M16" s="140"/>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B17" s="121">
+      <c r="B17" s="115">
         <v>-70</v>
       </c>
-      <c r="C17" s="122">
+      <c r="C17" s="116">
         <v>60</v>
       </c>
-      <c r="D17" s="123">
+      <c r="D17" s="117">
         <f t="shared" si="6"/>
         <v>-10</v>
       </c>
-      <c r="E17" s="124">
+      <c r="E17" s="118">
         <v>21412</v>
       </c>
-      <c r="F17" s="125">
+      <c r="F17" s="119">
         <f>10*LOG10(E17)</f>
         <v>43.306572347113942</v>
       </c>
-      <c r="G17" s="126">
+      <c r="G17" s="120">
         <v>238</v>
       </c>
-      <c r="J17" s="145"/>
-      <c r="K17" s="145"/>
-      <c r="L17" s="146"/>
-      <c r="M17" s="147"/>
+      <c r="J17" s="138"/>
+      <c r="K17" s="138"/>
+      <c r="L17" s="139"/>
+      <c r="M17" s="140"/>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B18" s="127">
+      <c r="B18" s="121">
         <v>-70</v>
       </c>
-      <c r="C18" s="128">
+      <c r="C18" s="122">
         <v>55</v>
       </c>
-      <c r="D18" s="129">
+      <c r="D18" s="123">
         <f t="shared" si="6"/>
         <v>-15</v>
       </c>
-      <c r="E18" s="130">
+      <c r="E18" s="124">
         <v>6420</v>
       </c>
-      <c r="F18" s="131">
+      <c r="F18" s="125">
         <f>10*LOG10(E18)</f>
         <v>38.075350280688532</v>
       </c>
-      <c r="G18" s="132">
+      <c r="G18" s="126">
         <v>117</v>
       </c>
-      <c r="J18" s="145"/>
-      <c r="K18" s="145"/>
-      <c r="L18" s="146"/>
-      <c r="M18" s="147"/>
+      <c r="J18" s="138"/>
+      <c r="K18" s="138"/>
+      <c r="L18" s="139"/>
+      <c r="M18" s="140"/>
     </row>
     <row r="19" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="133">
+      <c r="B19" s="127">
         <v>-70</v>
       </c>
-      <c r="C19" s="134">
+      <c r="C19" s="128">
         <v>50</v>
       </c>
-      <c r="D19" s="135">
+      <c r="D19" s="129">
         <f t="shared" si="6"/>
         <v>-20</v>
       </c>
-      <c r="E19" s="136">
+      <c r="E19" s="130">
         <v>2107</v>
       </c>
-      <c r="F19" s="137">
+      <c r="F19" s="131">
         <f>10*LOG10(E19)</f>
         <v>33.236645356080999</v>
       </c>
-      <c r="G19" s="138">
+      <c r="G19" s="132">
         <v>76</v>
       </c>
-      <c r="J19" s="145"/>
-      <c r="K19" s="145"/>
-      <c r="L19" s="146"/>
-      <c r="M19" s="147"/>
+      <c r="J19" s="138"/>
+      <c r="K19" s="138"/>
+      <c r="L19" s="139"/>
+      <c r="M19" s="140"/>
     </row>
     <row r="22" spans="2:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="144"/>
-      <c r="C22" s="144"/>
+      <c r="B22" s="137"/>
+      <c r="C22" s="137"/>
     </row>
     <row r="23" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="106" t="s">
+      <c r="B23" s="100" t="s">
         <v>42</v>
       </c>
-      <c r="C23" s="139" t="s">
+      <c r="C23" s="133" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B24" s="72">
+      <c r="B24" s="69">
         <v>5</v>
       </c>
-      <c r="C24" s="140">
+      <c r="C24" s="134">
         <f>(F6+F10)/2</f>
         <v>57.51449643412024</v>
       </c>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B25" s="74">
+      <c r="B25" s="71">
         <v>0</v>
       </c>
-      <c r="C25" s="141">
+      <c r="C25" s="135">
         <f>(F7+F11+F15)/3</f>
         <v>53.137894281262049</v>
       </c>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B26" s="74">
+      <c r="B26" s="71">
         <v>-5</v>
       </c>
-      <c r="C26" s="141">
+      <c r="C26" s="135">
         <f>(F8+F12+F16)/3</f>
         <v>48.118474175821056</v>
       </c>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B27" s="74">
+      <c r="B27" s="71">
         <v>-10</v>
       </c>
-      <c r="C27" s="141">
+      <c r="C27" s="135">
         <f>(F9+F13+F17)/3</f>
         <v>43.27472000811607</v>
       </c>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B28" s="74">
+      <c r="B28" s="71">
         <v>-15</v>
       </c>
-      <c r="C28" s="141">
+      <c r="C28" s="135">
         <f>(F14+F18)/2</f>
         <v>38.225301687592278</v>
       </c>
     </row>
     <row r="29" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="77">
+      <c r="B29" s="74">
         <v>-20</v>
       </c>
-      <c r="C29" s="142">
+      <c r="C29" s="136">
         <f>F19</f>
         <v>33.236645356080999</v>
       </c>

</xml_diff>